<commit_message>
finished the assembler and the transition to 5bit opcode
</commit_message>
<xml_diff>
--- a/Assembler/Instructions.xlsx
+++ b/Assembler/Instructions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
   <si>
     <t xml:space="preserve">INST</t>
   </si>
@@ -40,97 +40,139 @@
     <t xml:space="preserve">DST_REG</t>
   </si>
   <si>
-    <t xml:space="preserve">ADDRESSING_MODE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMM_VAL</t>
+    <t xml:space="preserve">NUM_ARGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGULAR</t>
   </si>
   <si>
     <t xml:space="preserve">MOV</t>
   </si>
   <si>
-    <t xml:space="preserve">0x0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGULAR</t>
+    <t xml:space="preserve">0x01</t>
   </si>
   <si>
     <t xml:space="preserve">ST</t>
   </si>
   <si>
-    <t xml:space="preserve">0x1</t>
+    <t xml:space="preserve">0x02</t>
   </si>
   <si>
     <t xml:space="preserve">PUSH</t>
   </si>
   <si>
-    <t xml:space="preserve">0x2</t>
+    <t xml:space="preserve">0x03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@0</t>
   </si>
   <si>
     <t xml:space="preserve">POP</t>
   </si>
   <si>
-    <t xml:space="preserve">0x3</t>
+    <t xml:space="preserve">0x04</t>
   </si>
   <si>
     <t xml:space="preserve">ADD</t>
   </si>
   <si>
-    <t xml:space="preserve">0x4</t>
+    <t xml:space="preserve">0x05</t>
   </si>
   <si>
     <t xml:space="preserve">ADDC</t>
   </si>
   <si>
-    <t xml:space="preserve">0x5</t>
+    <t xml:space="preserve">0x06</t>
   </si>
   <si>
     <t xml:space="preserve">SUB</t>
   </si>
   <si>
-    <t xml:space="preserve">0x6</t>
+    <t xml:space="preserve">0x07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x08</t>
   </si>
   <si>
     <t xml:space="preserve">SHR</t>
   </si>
   <si>
-    <t xml:space="preserve">0x8</t>
+    <t xml:space="preserve">0x09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0A</t>
   </si>
   <si>
     <t xml:space="preserve">RRC</t>
   </si>
   <si>
-    <t xml:space="preserve">0x9</t>
+    <t xml:space="preserve">0x0B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RLC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0C</t>
   </si>
   <si>
     <t xml:space="preserve">AND</t>
   </si>
   <si>
-    <t xml:space="preserve">0xA</t>
+    <t xml:space="preserve">0x0D</t>
   </si>
   <si>
     <t xml:space="preserve">OR</t>
   </si>
   <si>
-    <t xml:space="preserve">0xB</t>
+    <t xml:space="preserve">0x0E</t>
   </si>
   <si>
     <t xml:space="preserve">XOR</t>
   </si>
   <si>
-    <t xml:space="preserve">0xC</t>
+    <t xml:space="preserve">0x0F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x10</t>
   </si>
   <si>
     <t xml:space="preserve">CALL</t>
   </si>
   <si>
-    <t xml:space="preserve">0xE</t>
+    <t xml:space="preserve">0x11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x12</t>
   </si>
   <si>
     <t xml:space="preserve">JMP</t>
   </si>
   <si>
-    <t xml:space="preserve">0xF</t>
+    <t xml:space="preserve">0x13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HLT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x14</t>
   </si>
   <si>
     <t xml:space="preserve">dw</t>
@@ -158,36 +200,6 @@
   </si>
   <si>
     <t xml:space="preserve">JLS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HLT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIMULATED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x0010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0xFFFF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALTERNATIVE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RLC</t>
   </si>
 </sst>
 </file>
@@ -262,7 +274,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -273,10 +285,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -402,10 +410,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:XFD41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -415,10 +425,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.15"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -440,70 +449,78 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="XFC1" s="1"/>
+      <c r="XFD1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="0" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>0</v>
+      <c r="G5" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -514,9 +531,15 @@
         <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -528,10 +551,13 @@
         <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -542,10 +568,13 @@
         <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -556,10 +585,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -570,10 +602,13 @@
         <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -584,10 +619,13 @@
         <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -598,10 +636,13 @@
         <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -612,10 +653,13 @@
         <v>32</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -626,13 +670,13 @@
         <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E14" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -643,239 +687,305 @@
         <v>36</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>38</v>
+        <v>9</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>38</v>
+        <v>9</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F20" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>3</v>
       </c>
       <c r="F21" s="1" t="n">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F22" s="1" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F23" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F24" s="1" t="n">
-        <v>5</v>
+        <v>52</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F25" s="1" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F26" s="1" t="n">
-        <v>7</v>
+        <v>52</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>48</v>
+        <v>3</v>
+      </c>
+      <c r="F28" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>50</v>
+        <v>3</v>
+      </c>
+      <c r="F29" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G30" s="1" t="n">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="F30" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="D32" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="G32" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D33" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D34" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="D33" s="1"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D35" s="1"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D37" s="1"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D41" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
fixed some instructions, added highlight for neovim
first try with kicad
</commit_message>
<xml_diff>
--- a/Assembler/Instructions.xlsx
+++ b/Assembler/Instructions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="62">
   <si>
     <t xml:space="preserve">INST</t>
   </si>
@@ -200,6 +200,12 @@
   </si>
   <si>
     <t xml:space="preserve">JLS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIMULATED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#0x0010</t>
   </si>
 </sst>
 </file>
@@ -415,7 +421,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -465,7 +471,7 @@
       <c r="D2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -482,7 +488,7 @@
       <c r="D3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -499,7 +505,7 @@
       <c r="D4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -519,7 +525,7 @@
       <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -539,7 +545,7 @@
       <c r="E6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -556,7 +562,7 @@
       <c r="D7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -573,7 +579,7 @@
       <c r="D8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -590,7 +596,7 @@
       <c r="D9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -607,7 +613,7 @@
       <c r="D10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -624,7 +630,7 @@
       <c r="D11" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -641,7 +647,7 @@
       <c r="D12" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -658,7 +664,7 @@
       <c r="D13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -675,7 +681,7 @@
       <c r="D14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -692,7 +698,7 @@
       <c r="D15" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -709,7 +715,7 @@
       <c r="D16" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -726,7 +732,7 @@
       <c r="D17" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -743,7 +749,7 @@
       <c r="D18" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -763,7 +769,7 @@
       <c r="E19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="G19" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -786,7 +792,7 @@
       <c r="F20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="G20" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -806,7 +812,7 @@
       <c r="F21" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="G21" s="0" t="n">
+      <c r="G21" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -826,7 +832,7 @@
       <c r="F22" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G22" s="0" t="n">
+      <c r="G22" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -837,7 +843,7 @@
       <c r="C24" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G24" s="0" t="n">
+      <c r="G24" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -848,7 +854,7 @@
       <c r="C25" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="G25" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -868,7 +874,7 @@
       <c r="F27" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G27" s="0" t="n">
+      <c r="G27" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -888,7 +894,7 @@
       <c r="F28" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="G28" s="0" t="n">
+      <c r="G28" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -908,7 +914,7 @@
       <c r="F29" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G29" s="0" t="n">
+      <c r="G29" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -928,7 +934,7 @@
       <c r="F30" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="G30" s="0" t="n">
+      <c r="G30" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -948,7 +954,7 @@
       <c r="F31" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="G31" s="0" t="n">
+      <c r="G31" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -968,15 +974,42 @@
       <c r="F32" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G32" s="0" t="n">
+      <c r="G32" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D33" s="1"/>
     </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D35" s="1"/>
+      <c r="A35" s="0"/>
+      <c r="B35" s="0"/>
+      <c r="C35" s="0"/>
+      <c r="E35" s="0"/>
+      <c r="F35" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D37" s="1"/>

</xml_diff>